<commit_message>
Raspberry Pi confirm of parts list amend.
</commit_message>
<xml_diff>
--- a/etc/PrintPupper_design.xlsx
+++ b/etc/PrintPupper_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2fc58c125a83494/OneDriveWork2/DogRobot_2/git/PrintPupper/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{9CC67CED-55A3-4FF6-B430-CC58A595A9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C015C163-E13B-4DE1-86E0-CDE208B141B8}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{9CC67CED-55A3-4FF6-B430-CC58A595A9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15BAA9BF-A843-47B8-B01A-265225E4DEBD}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="234">
   <si>
     <t>Front Right</t>
     <phoneticPr fontId="1"/>
@@ -740,25 +740,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Raspberry Pi "3" or "4" or "Zero W"</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ラズベリーパイ 3または4またはZero W</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>※ Zero2 W is ok</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>※Zero2 Wでも可</t>
-    <rPh sb="10" eb="11">
-      <t>カ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Battery バッテリー</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1079,10 +1060,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Zero</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>エレコム ワイヤレス ゲームパッド JC-U3912TBK</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1238,6 +1215,28 @@
   </si>
   <si>
     <t>a robots</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Raspberry Pi "3" or "4" or "Zero 2 W"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ラズベリーパイ 3または4またはZero 2 W</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※ Zero W is NG</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※Zero W は動作不可</t>
+    <rPh sb="9" eb="11">
+      <t>ドウサ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>フカ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1249,7 +1248,7 @@
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="176" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1329,6 +1328,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Yu Gothic"/>
@@ -1577,7 +1584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1666,6 +1673,7 @@
     <xf numFmtId="176" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -4237,7 +4245,7 @@
   <sheetData>
     <row r="2" spans="2:24" ht="19.5" thickBot="1">
       <c r="B2" s="40" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -4269,11 +4277,11 @@
     </row>
     <row r="4" spans="2:24">
       <c r="B4" s="7" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -4284,13 +4292,13 @@
         <v>42000</v>
       </c>
       <c r="J4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="X4" s="11"/>
     </row>
     <row r="5" spans="2:24">
       <c r="B5" s="10" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="45" t="s">
@@ -4305,7 +4313,7 @@
         <v>4368</v>
       </c>
       <c r="J5" s="56" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="K5" s="47"/>
       <c r="L5" s="47"/>
@@ -4328,7 +4336,7 @@
       </c>
       <c r="J6" s="46"/>
       <c r="K6" s="73" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="L6" s="46"/>
       <c r="M6" s="58"/>
@@ -4349,7 +4357,7 @@
         <v>1564</v>
       </c>
       <c r="J7" s="60" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="K7" s="42"/>
       <c r="L7" s="42"/>
@@ -4375,7 +4383,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="10" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I9" s="19"/>
       <c r="X9" s="11"/>
@@ -4384,7 +4392,7 @@
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="38" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I10" s="19"/>
       <c r="X10" s="11"/>
@@ -4393,7 +4401,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="39" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E11" s="74"/>
       <c r="F11" s="13"/>
@@ -4413,7 +4421,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I12" s="55">
         <f>SUM(I4:I11)</f>
@@ -4423,10 +4431,10 @@
     </row>
     <row r="13" spans="2:24">
       <c r="B13" s="78" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H13" s="79" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="I13" s="37"/>
       <c r="X13" s="11"/>
@@ -4460,19 +4468,19 @@
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
       <c r="I15" s="25" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
       <c r="L15" s="25"/>
       <c r="M15" s="25" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="25" t="s">
@@ -4482,14 +4490,14 @@
         <v>85</v>
       </c>
       <c r="Q15" s="27" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="R15" s="28" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="S15" s="29"/>
       <c r="T15" s="25" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="U15" s="25"/>
       <c r="V15" s="25"/>
@@ -4498,13 +4506,13 @@
     </row>
     <row r="16" spans="2:24">
       <c r="B16" s="10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="M16">
         <f>O16*4+P16*2</f>
@@ -4527,10 +4535,10 @@
     <row r="17" spans="2:24">
       <c r="B17" s="10"/>
       <c r="E17" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I17" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="10"/>
@@ -4885,13 +4893,13 @@
       <c r="C28" s="46"/>
       <c r="D28" s="46"/>
       <c r="E28" s="46" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F28" s="46"/>
       <c r="G28" s="46"/>
       <c r="H28" s="46"/>
       <c r="I28" s="46" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J28" s="46"/>
       <c r="K28" s="46"/>
@@ -4947,7 +4955,7 @@
       <c r="G30" s="46"/>
       <c r="H30" s="46"/>
       <c r="I30" s="46" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J30" s="46"/>
       <c r="K30" s="46"/>
@@ -4982,7 +4990,7 @@
       <c r="G31" s="46"/>
       <c r="H31" s="46"/>
       <c r="I31" s="46" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J31" s="46"/>
       <c r="K31" s="46"/>
@@ -5032,13 +5040,13 @@
       <c r="C33" s="46"/>
       <c r="D33" s="46"/>
       <c r="E33" s="46" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F33" s="46"/>
       <c r="G33" s="46"/>
       <c r="H33" s="46"/>
       <c r="I33" s="46" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J33" s="46"/>
       <c r="K33" s="46"/>
@@ -5141,18 +5149,18 @@
     </row>
     <row r="37" spans="2:24">
       <c r="B37" s="53" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C37" s="46"/>
       <c r="D37" s="46"/>
       <c r="E37" s="46" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F37" s="46"/>
       <c r="G37" s="46"/>
       <c r="H37" s="46"/>
       <c r="I37" s="46" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J37" s="46"/>
       <c r="K37" s="46"/>
@@ -5214,7 +5222,7 @@
       <c r="O39" s="70"/>
       <c r="P39" s="71"/>
       <c r="Q39" s="69" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="R39" s="72">
         <f>SUM(R19:R37)</f>
@@ -5248,12 +5256,12 @@
       <c r="O40" s="46"/>
       <c r="P40" s="58"/>
       <c r="Q40" s="53" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="R40" s="58"/>
       <c r="S40" s="10"/>
       <c r="T40" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="X40" s="11"/>
     </row>
@@ -5285,12 +5293,12 @@
       <c r="O41" s="46"/>
       <c r="P41" s="58"/>
       <c r="Q41" s="53" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="R41" s="58"/>
       <c r="S41" s="10"/>
       <c r="T41" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="X41" s="11"/>
     </row>
@@ -5317,12 +5325,12 @@
       <c r="O42" s="46"/>
       <c r="P42" s="58"/>
       <c r="Q42" s="53" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="R42" s="58"/>
       <c r="S42" s="10"/>
       <c r="T42" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="X42" s="11"/>
     </row>
@@ -5349,12 +5357,12 @@
       <c r="O43" s="46"/>
       <c r="P43" s="58"/>
       <c r="Q43" s="53" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="R43" s="58"/>
       <c r="S43" s="10"/>
       <c r="T43" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="X43" s="11"/>
     </row>
@@ -5384,7 +5392,7 @@
       <c r="R44" s="58"/>
       <c r="S44" s="10"/>
       <c r="T44" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="X44" s="11"/>
     </row>
@@ -5399,7 +5407,7 @@
       <c r="G45" s="46"/>
       <c r="H45" s="46"/>
       <c r="I45" s="46" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="J45" s="46"/>
       <c r="K45" s="46"/>
@@ -5414,7 +5422,7 @@
       <c r="R45" s="58"/>
       <c r="S45" s="10"/>
       <c r="T45" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="X45" s="11"/>
     </row>
@@ -5429,7 +5437,7 @@
       <c r="G46" s="46"/>
       <c r="H46" s="46"/>
       <c r="I46" s="46" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J46" s="46"/>
       <c r="K46" s="46"/>
@@ -5444,7 +5452,7 @@
       <c r="R46" s="58"/>
       <c r="S46" s="10"/>
       <c r="T46" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="X46" s="11"/>
     </row>
@@ -5459,7 +5467,7 @@
       <c r="G47" s="46"/>
       <c r="H47" s="46"/>
       <c r="I47" s="46" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J47" s="46"/>
       <c r="K47" s="46"/>
@@ -5474,7 +5482,7 @@
       <c r="R47" s="58"/>
       <c r="S47" s="10"/>
       <c r="T47" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="X47" s="11"/>
     </row>
@@ -5504,7 +5512,7 @@
       <c r="R48" s="58"/>
       <c r="S48" s="10"/>
       <c r="T48" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="X48" s="11"/>
     </row>
@@ -5534,7 +5542,7 @@
       <c r="R49" s="58"/>
       <c r="S49" s="10"/>
       <c r="T49" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="X49" s="11"/>
     </row>
@@ -5564,7 +5572,7 @@
       <c r="R50" s="58"/>
       <c r="S50" s="10"/>
       <c r="T50" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="X50" s="11"/>
     </row>
@@ -5594,7 +5602,7 @@
       <c r="R51" s="58"/>
       <c r="S51" s="10"/>
       <c r="T51" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="X51" s="11"/>
     </row>
@@ -5624,7 +5632,7 @@
       <c r="R52" s="58"/>
       <c r="S52" s="10"/>
       <c r="T52" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="X52" s="11"/>
     </row>
@@ -5666,7 +5674,7 @@
       <c r="O54" s="70"/>
       <c r="P54" s="71"/>
       <c r="Q54" s="69" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="R54" s="72">
         <v>2800</v>
@@ -5711,7 +5719,7 @@
       </c>
       <c r="S55" s="15"/>
       <c r="T55" s="16" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="U55" s="16"/>
       <c r="V55" s="16"/>
@@ -5754,13 +5762,13 @@
       <c r="D57" s="42"/>
       <c r="E57" s="42"/>
       <c r="F57" s="42" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G57" s="42"/>
       <c r="H57" s="42"/>
       <c r="I57" s="42"/>
       <c r="J57" s="42" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="K57" s="42"/>
       <c r="L57" s="42"/>
@@ -5885,13 +5893,13 @@
       <c r="C62" s="42"/>
       <c r="D62" s="42"/>
       <c r="E62" s="42" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F62" s="42"/>
       <c r="G62" s="42"/>
       <c r="H62" s="42"/>
       <c r="I62" s="42" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J62" s="42"/>
       <c r="K62" s="42"/>
@@ -5915,13 +5923,13 @@
       <c r="C63" s="42"/>
       <c r="D63" s="42"/>
       <c r="E63" s="42" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F63" s="42"/>
       <c r="G63" s="42"/>
       <c r="H63" s="42"/>
       <c r="I63" s="42" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J63" s="42"/>
       <c r="K63" s="42"/>
@@ -5945,13 +5953,13 @@
       <c r="C64" s="42"/>
       <c r="D64" s="42"/>
       <c r="E64" s="42" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F64" s="42"/>
       <c r="G64" s="42"/>
       <c r="H64" s="42"/>
       <c r="I64" s="42" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J64" s="42"/>
       <c r="K64" s="42"/>
@@ -6005,13 +6013,13 @@
       <c r="C66" s="42"/>
       <c r="D66" s="42"/>
       <c r="E66" s="42" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F66" s="42"/>
       <c r="G66" s="42"/>
       <c r="H66" s="42"/>
       <c r="I66" s="42" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J66" s="42"/>
       <c r="K66" s="42"/>
@@ -6126,7 +6134,7 @@
       <c r="O70" s="65"/>
       <c r="P70" s="66"/>
       <c r="Q70" s="64" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="R70" s="67">
         <f>SUM(R55:R68)</f>
@@ -6138,16 +6146,16 @@
         <v>143</v>
       </c>
       <c r="E71" t="s">
-        <v>144</v>
+        <v>230</v>
       </c>
       <c r="I71" t="s">
-        <v>145</v>
+        <v>231</v>
       </c>
       <c r="M71">
         <v>1</v>
       </c>
       <c r="P71" s="11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="Q71" s="10"/>
       <c r="R71" s="19">
@@ -6156,18 +6164,16 @@
     </row>
     <row r="72" spans="2:18">
       <c r="B72" s="10"/>
-      <c r="F72" t="s">
-        <v>146</v>
-      </c>
-      <c r="J72" t="s">
-        <v>147</v>
-      </c>
-      <c r="O72" t="s">
-        <v>213</v>
-      </c>
-      <c r="P72" s="11" t="s">
-        <v>211</v>
-      </c>
+      <c r="F72" s="80" t="s">
+        <v>232</v>
+      </c>
+      <c r="G72" s="80"/>
+      <c r="H72" s="80"/>
+      <c r="I72" s="80"/>
+      <c r="J72" s="80" t="s">
+        <v>233</v>
+      </c>
+      <c r="P72" s="11"/>
       <c r="Q72" s="10"/>
       <c r="R72" s="19">
         <v>4000</v>
@@ -6181,13 +6187,13 @@
     </row>
     <row r="74" spans="2:18">
       <c r="B74" s="10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E74" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I74" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="M74">
         <v>1</v>
@@ -6201,10 +6207,10 @@
     <row r="75" spans="2:18">
       <c r="B75" s="10"/>
       <c r="C75" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E75" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P75" s="11"/>
       <c r="Q75" s="10"/>
@@ -6213,10 +6219,10 @@
     <row r="76" spans="2:18">
       <c r="B76" s="10"/>
       <c r="C76" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E76" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="P76" s="11"/>
       <c r="Q76" s="10"/>
@@ -6225,10 +6231,10 @@
     <row r="77" spans="2:18">
       <c r="B77" s="10"/>
       <c r="F77" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I77" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="P77" s="11"/>
       <c r="Q77" s="10"/>
@@ -6315,12 +6321,12 @@
     </row>
     <row r="83" spans="2:18">
       <c r="B83" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
       <c r="E83" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J83" s="8"/>
       <c r="K83" s="8"/>
@@ -6331,7 +6337,7 @@
       <c r="N83" s="8"/>
       <c r="O83" s="8"/>
       <c r="P83" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q83" s="7"/>
       <c r="R83" s="19">
@@ -6341,19 +6347,19 @@
     <row r="84" spans="2:18">
       <c r="B84" s="10"/>
       <c r="E84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I84" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="M84">
         <v>1</v>
       </c>
       <c r="O84" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P84" s="11" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="Q84" s="18"/>
       <c r="R84" s="19">
@@ -6363,10 +6369,10 @@
     <row r="85" spans="2:18">
       <c r="B85" s="10"/>
       <c r="E85" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I85" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P85" s="11"/>
       <c r="Q85" s="10"/>
@@ -6395,7 +6401,7 @@
       <c r="O87" s="23"/>
       <c r="P87" s="24"/>
       <c r="Q87" s="29" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="R87" s="30">
         <f>R72+R74+R83</f>
@@ -6799,7 +6805,7 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>